<commit_message>
Update Planilla Petreles gigantes para Martina.xlsx
</commit_message>
<xml_diff>
--- a/Planilla Petreles gigantes para Martina.xlsx
+++ b/Planilla Petreles gigantes para Martina.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martu\Documents\GitHub\TP_FINAL_BIOME_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E26160E-1972-42A4-B606-C59940031D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4FBCE2-A73D-47AD-B965-CEB9045A4B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AF24A696-3648-44CB-BE4D-C80E224E0C6C}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="106">
   <si>
     <t>Tendencia poblacional de las colonias de Petrel gigante de Punta Duthoit</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>Colonia A: + cerca a la base, pero esta en altura (dentro de ZAEP)</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -544,16 +547,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2328,10 +2322,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB98568-9EA6-4C5E-939D-E5F3C641C618}">
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,7 +2338,7 @@
     <col min="11" max="11" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>82</v>
       </c>
@@ -2370,7 +2364,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>35</v>
       </c>
@@ -2393,7 +2387,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>81</v>
@@ -2411,7 +2405,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>81</v>
@@ -2429,7 +2423,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>81</v>
@@ -2447,7 +2441,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>81</v>
@@ -2465,7 +2459,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>81</v>
@@ -2480,7 +2474,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="31" t="s">
         <v>81</v>
@@ -2495,31 +2489,30 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>73</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="33" t="s">
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9">
         <v>119</v>
       </c>
       <c r="F9">
         <v>7</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9">
         <v>2016</v>
       </c>
-      <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" t="s">
         <v>81</v>
@@ -2527,10 +2520,9 @@
       <c r="C10" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10">
         <v>16</v>
       </c>
-      <c r="E10" s="34"/>
       <c r="F10">
         <v>25</v>
       </c>
@@ -2538,7 +2530,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>81</v>
@@ -2546,10 +2538,9 @@
       <c r="C11" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11">
         <v>18</v>
       </c>
-      <c r="E11" s="34"/>
       <c r="F11">
         <v>4</v>
       </c>
@@ -2557,7 +2548,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>81</v>
@@ -2565,10 +2556,9 @@
       <c r="C12" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="34">
-        <v>0</v>
-      </c>
-      <c r="E12" s="34"/>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="F12">
         <v>6</v>
       </c>
@@ -2576,17 +2566,16 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13">
         <v>35</v>
       </c>
-      <c r="E13" s="34"/>
       <c r="F13">
         <v>28</v>
       </c>
@@ -2594,17 +2583,16 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" s="34"/>
       <c r="F14">
         <v>45</v>
       </c>
@@ -2612,7 +2600,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="31" t="s">
         <v>81</v>
@@ -2630,8 +2618,11 @@
       <c r="G15" s="31">
         <v>2016</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>70</v>
       </c>
@@ -2641,27 +2632,24 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16">
         <v>6</v>
       </c>
-      <c r="E16" s="34"/>
       <c r="G16">
         <v>2017</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="33" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17">
         <v>13</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="33"/>
       <c r="G17">
         <v>2017</v>
       </c>
@@ -2673,10 +2661,9 @@
       <c r="C18" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18">
         <v>14</v>
       </c>
-      <c r="E18" s="34"/>
       <c r="G18">
         <v>2017</v>
       </c>
@@ -2691,10 +2678,9 @@
       <c r="C19" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19">
         <v>8</v>
       </c>
-      <c r="E19" s="34"/>
       <c r="G19">
         <v>2017</v>
       </c>
@@ -2709,10 +2695,9 @@
       <c r="C20" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20">
         <v>26</v>
       </c>
-      <c r="E20" s="34"/>
       <c r="G20">
         <v>2017</v>
       </c>
@@ -2727,10 +2712,9 @@
       <c r="C21" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="34"/>
       <c r="G21">
         <v>2017</v>
       </c>
@@ -2768,10 +2752,10 @@
       <c r="C23" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23">
         <v>11</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23">
         <v>67</v>
       </c>
       <c r="F23">
@@ -2791,11 +2775,10 @@
       <c r="C24" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="33">
+      <c r="F24">
         <v>22</v>
       </c>
       <c r="G24">
@@ -2806,17 +2789,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="33" t="s">
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25">
         <v>9</v>
       </c>
-      <c r="E25" s="34"/>
       <c r="F25">
         <v>10</v>
       </c>
@@ -2834,10 +2815,9 @@
       <c r="C26" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="34"/>
       <c r="F26">
         <v>6</v>
       </c>
@@ -2855,10 +2835,9 @@
       <c r="C27" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="34">
-        <v>0</v>
-      </c>
-      <c r="E27" s="34"/>
+      <c r="D27">
+        <v>0</v>
+      </c>
       <c r="F27">
         <v>13</v>
       </c>
@@ -2873,10 +2852,9 @@
       <c r="C28" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28" s="34"/>
       <c r="F28">
         <v>2</v>
       </c>
@@ -2892,10 +2870,10 @@
       <c r="C29" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="31">
         <v>7</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="31">
         <v>4</v>
       </c>
@@ -2913,13 +2891,13 @@
       <c r="C30" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30">
         <v>52</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30">
         <v>14</v>
       </c>
       <c r="G30">
@@ -2933,11 +2911,10 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34">
+      <c r="F31">
         <v>2</v>
       </c>
       <c r="G31">
@@ -2951,11 +2928,10 @@
       <c r="C32" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32">
         <v>3</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34">
+      <c r="F32">
         <v>7</v>
       </c>
       <c r="G32">
@@ -2969,11 +2945,10 @@
       <c r="C33" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="34">
-        <v>0</v>
-      </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>10</v>
       </c>
       <c r="G33">
@@ -2987,11 +2962,10 @@
       <c r="C34" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="34">
-        <v>0</v>
-      </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="F34">
         <v>12</v>
       </c>
       <c r="G34">
@@ -3005,11 +2979,10 @@
       <c r="C35" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="34">
-        <v>0</v>
-      </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <v>2</v>
       </c>
       <c r="G35">
@@ -3045,11 +3018,9 @@
       <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37">
         <v>3</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
       <c r="G37">
         <v>2020</v>
       </c>
@@ -3061,11 +3032,9 @@
       <c r="C38" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="34">
-        <v>0</v>
-      </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="D38">
+        <v>0</v>
+      </c>
       <c r="G38">
         <v>2020</v>
       </c>
@@ -3077,11 +3046,9 @@
       <c r="C39" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="34">
-        <v>0</v>
-      </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="G39">
         <v>2020</v>
       </c>
@@ -3093,11 +3060,9 @@
       <c r="C40" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="34">
-        <v>0</v>
-      </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
+      <c r="D40">
+        <v>0</v>
+      </c>
       <c r="G40">
         <v>2020</v>
       </c>
@@ -3109,11 +3074,9 @@
       <c r="C41" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="34">
-        <v>0</v>
-      </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
+      <c r="D41">
+        <v>0</v>
+      </c>
       <c r="G41">
         <v>2020</v>
       </c>
@@ -3125,11 +3088,9 @@
       <c r="C42" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42">
         <v>1</v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
       <c r="G42">
         <v>2020</v>
       </c>
@@ -3142,10 +3103,10 @@
       <c r="C43" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="37">
+      <c r="D43" s="31">
         <v>9</v>
       </c>
-      <c r="E43" s="37"/>
+      <c r="E43" s="31"/>
       <c r="F43" s="31"/>
       <c r="G43" s="31">
         <v>2020</v>
@@ -3161,13 +3122,13 @@
       <c r="C44" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="34">
-        <v>0</v>
-      </c>
-      <c r="E44" s="34">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
         <v>65</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44">
         <v>25</v>
       </c>
       <c r="G44">
@@ -3181,11 +3142,10 @@
       <c r="C45" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="34">
-        <v>0</v>
-      </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
@@ -3199,11 +3159,10 @@
       <c r="C46" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="34">
-        <v>0</v>
-      </c>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>5</v>
       </c>
       <c r="G46">
@@ -3217,11 +3176,10 @@
       <c r="C47" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="34">
-        <v>0</v>
-      </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>20</v>
       </c>
       <c r="G47">
@@ -3235,11 +3193,10 @@
       <c r="C48" t="s">
         <v>90</v>
       </c>
-      <c r="D48" s="34">
-        <v>0</v>
-      </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
@@ -3253,11 +3210,10 @@
       <c r="C49" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="34">
-        <v>0</v>
-      </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
@@ -3293,13 +3249,13 @@
       <c r="C51" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="34">
+      <c r="D51">
         <v>10</v>
       </c>
-      <c r="E51" s="34">
+      <c r="E51">
         <v>74</v>
       </c>
-      <c r="F51" s="34">
+      <c r="F51">
         <v>18</v>
       </c>
       <c r="G51">
@@ -3313,11 +3269,10 @@
       <c r="C52" t="s">
         <v>85</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52">
         <v>1</v>
       </c>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34">
+      <c r="F52">
         <v>4</v>
       </c>
       <c r="G52">
@@ -3331,11 +3286,10 @@
       <c r="C53" t="s">
         <v>86</v>
       </c>
-      <c r="D53" s="34">
+      <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34">
+      <c r="F53">
         <v>12</v>
       </c>
       <c r="G53">
@@ -3349,11 +3303,10 @@
       <c r="C54" t="s">
         <v>87</v>
       </c>
-      <c r="D54" s="34">
-        <v>0</v>
-      </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="F54">
         <v>1</v>
       </c>
       <c r="G54">
@@ -3367,11 +3320,10 @@
       <c r="C55" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="34">
-        <v>0</v>
-      </c>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="F55">
         <v>13</v>
       </c>
       <c r="G55">
@@ -3385,11 +3337,10 @@
       <c r="C56" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="34">
+      <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34">
+      <c r="F56">
         <v>3</v>
       </c>
       <c r="G56">
@@ -3425,13 +3376,13 @@
       <c r="C58" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="34">
+      <c r="D58">
         <v>7</v>
       </c>
-      <c r="E58" s="34">
+      <c r="E58">
         <v>65</v>
       </c>
-      <c r="F58" s="34">
+      <c r="F58">
         <v>21</v>
       </c>
       <c r="G58">
@@ -3445,11 +3396,10 @@
       <c r="C59" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="34">
-        <v>0</v>
-      </c>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="F59">
         <v>6</v>
       </c>
       <c r="G59">
@@ -3463,11 +3413,10 @@
       <c r="C60" t="s">
         <v>86</v>
       </c>
-      <c r="D60" s="34">
-        <v>0</v>
-      </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="F60">
         <v>2</v>
       </c>
       <c r="G60">
@@ -3481,11 +3430,10 @@
       <c r="C61" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="34">
-        <v>0</v>
-      </c>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34">
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="F61">
         <v>3</v>
       </c>
       <c r="G61">
@@ -3499,11 +3447,10 @@
       <c r="C62" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="34">
-        <v>0</v>
-      </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="F62">
         <v>3</v>
       </c>
       <c r="G62">
@@ -3517,11 +3464,10 @@
       <c r="C63" t="s">
         <v>88</v>
       </c>
-      <c r="D63" s="34">
-        <v>0</v>
-      </c>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34">
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="F63">
         <v>4</v>
       </c>
       <c r="G63">
@@ -3557,10 +3503,10 @@
       <c r="C65" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="34">
-        <v>0</v>
-      </c>
-      <c r="E65" s="34">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
         <v>36</v>
       </c>
       <c r="F65">
@@ -3577,10 +3523,9 @@
       <c r="C66" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="34">
-        <v>0</v>
-      </c>
-      <c r="E66" s="34"/>
+      <c r="D66">
+        <v>0</v>
+      </c>
       <c r="F66">
         <v>2</v>
       </c>
@@ -3595,10 +3540,9 @@
       <c r="C67" t="s">
         <v>86</v>
       </c>
-      <c r="D67" s="34">
-        <v>0</v>
-      </c>
-      <c r="E67" s="34"/>
+      <c r="D67">
+        <v>0</v>
+      </c>
       <c r="F67">
         <v>1</v>
       </c>
@@ -3613,10 +3557,9 @@
       <c r="C68" t="s">
         <v>87</v>
       </c>
-      <c r="D68" s="34">
-        <v>0</v>
-      </c>
-      <c r="E68" s="34"/>
+      <c r="D68">
+        <v>0</v>
+      </c>
       <c r="F68">
         <v>1</v>
       </c>
@@ -3631,10 +3574,9 @@
       <c r="C69" t="s">
         <v>90</v>
       </c>
-      <c r="D69" s="34">
-        <v>0</v>
-      </c>
-      <c r="E69" s="34"/>
+      <c r="D69">
+        <v>0</v>
+      </c>
       <c r="F69">
         <v>1</v>
       </c>
@@ -3649,10 +3591,9 @@
       <c r="C70" t="s">
         <v>88</v>
       </c>
-      <c r="D70" s="34">
-        <v>0</v>
-      </c>
-      <c r="E70" s="34"/>
+      <c r="D70">
+        <v>0</v>
+      </c>
       <c r="F70">
         <v>4</v>
       </c>
@@ -3689,10 +3630,10 @@
       <c r="C72" t="s">
         <v>84</v>
       </c>
-      <c r="D72" s="34">
-        <v>0</v>
-      </c>
-      <c r="E72" s="34">
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
         <v>33</v>
       </c>
       <c r="F72">
@@ -3709,10 +3650,9 @@
       <c r="C73" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="34">
-        <v>0</v>
-      </c>
-      <c r="E73" s="34"/>
+      <c r="D73">
+        <v>0</v>
+      </c>
       <c r="F73">
         <v>0</v>
       </c>
@@ -3727,10 +3667,9 @@
       <c r="C74" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="34">
-        <v>0</v>
-      </c>
-      <c r="E74" s="34"/>
+      <c r="D74">
+        <v>0</v>
+      </c>
       <c r="F74">
         <v>0</v>
       </c>
@@ -3745,10 +3684,9 @@
       <c r="C75" t="s">
         <v>87</v>
       </c>
-      <c r="D75" s="34">
-        <v>0</v>
-      </c>
-      <c r="E75" s="34"/>
+      <c r="D75">
+        <v>0</v>
+      </c>
       <c r="F75">
         <v>0</v>
       </c>
@@ -3763,10 +3701,9 @@
       <c r="C76" t="s">
         <v>90</v>
       </c>
-      <c r="D76" s="34">
-        <v>0</v>
-      </c>
-      <c r="E76" s="34"/>
+      <c r="D76">
+        <v>0</v>
+      </c>
       <c r="F76">
         <v>0</v>
       </c>
@@ -3781,10 +3718,9 @@
       <c r="C77" t="s">
         <v>88</v>
       </c>
-      <c r="D77" s="34">
-        <v>0</v>
-      </c>
-      <c r="E77" s="34"/>
+      <c r="D77">
+        <v>0</v>
+      </c>
       <c r="F77">
         <v>1</v>
       </c>
@@ -3800,10 +3736,10 @@
       <c r="C78" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D78" s="37">
+      <c r="D78" s="31">
         <v>13</v>
       </c>
-      <c r="E78" s="37"/>
+      <c r="E78" s="31"/>
       <c r="F78" s="31">
         <v>19</v>
       </c>
@@ -3824,7 +3760,7 @@
       <c r="E79">
         <v>12</v>
       </c>
-      <c r="G79" s="34">
+      <c r="G79">
         <v>2015</v>
       </c>
     </row>
@@ -3835,7 +3771,7 @@
       <c r="C80" t="s">
         <v>91</v>
       </c>
-      <c r="G80" s="34">
+      <c r="G80">
         <v>2015</v>
       </c>
     </row>
@@ -3846,7 +3782,7 @@
       <c r="C81" t="s">
         <v>92</v>
       </c>
-      <c r="G81" s="34">
+      <c r="G81">
         <v>2015</v>
       </c>
     </row>
@@ -3857,7 +3793,7 @@
       <c r="C82">
         <v>3</v>
       </c>
-      <c r="G82" s="34">
+      <c r="G82">
         <v>2015</v>
       </c>
     </row>
@@ -3868,7 +3804,7 @@
       <c r="C83">
         <v>4</v>
       </c>
-      <c r="G83" s="34">
+      <c r="G83">
         <v>2015</v>
       </c>
     </row>
@@ -3879,7 +3815,7 @@
       <c r="C84">
         <v>5</v>
       </c>
-      <c r="G84" s="34">
+      <c r="G84">
         <v>2015</v>
       </c>
     </row>
@@ -3894,7 +3830,7 @@
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
       <c r="F85" s="31"/>
-      <c r="G85" s="37">
+      <c r="G85" s="31">
         <v>2015</v>
       </c>
     </row>
@@ -3911,7 +3847,7 @@
       <c r="E86">
         <v>11</v>
       </c>
-      <c r="G86" s="34">
+      <c r="G86">
         <v>2016</v>
       </c>
     </row>
@@ -3922,7 +3858,7 @@
       <c r="C87" t="s">
         <v>91</v>
       </c>
-      <c r="G87" s="34">
+      <c r="G87">
         <v>2016</v>
       </c>
     </row>
@@ -3933,7 +3869,7 @@
       <c r="C88" t="s">
         <v>92</v>
       </c>
-      <c r="G88" s="34">
+      <c r="G88">
         <v>2016</v>
       </c>
     </row>
@@ -3944,7 +3880,7 @@
       <c r="C89">
         <v>3</v>
       </c>
-      <c r="G89" s="34">
+      <c r="G89">
         <v>2016</v>
       </c>
     </row>
@@ -3955,7 +3891,7 @@
       <c r="C90">
         <v>4</v>
       </c>
-      <c r="G90" s="34">
+      <c r="G90">
         <v>2016</v>
       </c>
     </row>
@@ -3966,7 +3902,7 @@
       <c r="C91">
         <v>5</v>
       </c>
-      <c r="G91" s="34">
+      <c r="G91">
         <v>2016</v>
       </c>
     </row>
@@ -3981,7 +3917,7 @@
       <c r="D92" s="31"/>
       <c r="E92" s="31"/>
       <c r="F92" s="31"/>
-      <c r="G92" s="37">
+      <c r="G92" s="31">
         <v>2016</v>
       </c>
     </row>
@@ -3998,7 +3934,7 @@
       <c r="D93">
         <v>15</v>
       </c>
-      <c r="G93" s="34">
+      <c r="G93">
         <v>2017</v>
       </c>
     </row>
@@ -4009,7 +3945,7 @@
       <c r="C94" t="s">
         <v>91</v>
       </c>
-      <c r="G94" s="34">
+      <c r="G94">
         <v>2017</v>
       </c>
     </row>
@@ -4020,7 +3956,7 @@
       <c r="C95" t="s">
         <v>92</v>
       </c>
-      <c r="G95" s="34">
+      <c r="G95">
         <v>2017</v>
       </c>
     </row>
@@ -4031,7 +3967,7 @@
       <c r="C96">
         <v>3</v>
       </c>
-      <c r="G96" s="34">
+      <c r="G96">
         <v>2017</v>
       </c>
     </row>
@@ -4042,7 +3978,7 @@
       <c r="C97">
         <v>4</v>
       </c>
-      <c r="G97" s="34">
+      <c r="G97">
         <v>2017</v>
       </c>
     </row>
@@ -4053,7 +3989,7 @@
       <c r="C98">
         <v>5</v>
       </c>
-      <c r="G98" s="34">
+      <c r="G98">
         <v>2017</v>
       </c>
     </row>
@@ -4068,7 +4004,7 @@
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
       <c r="F99" s="31"/>
-      <c r="G99" s="37">
+      <c r="G99" s="31">
         <v>2017</v>
       </c>
     </row>
@@ -4082,7 +4018,7 @@
       <c r="C100">
         <v>1</v>
       </c>
-      <c r="G100" s="34">
+      <c r="G100">
         <v>2018</v>
       </c>
     </row>
@@ -4093,7 +4029,7 @@
       <c r="C101" t="s">
         <v>91</v>
       </c>
-      <c r="G101" s="34">
+      <c r="G101">
         <v>2018</v>
       </c>
     </row>
@@ -4104,7 +4040,7 @@
       <c r="C102" t="s">
         <v>92</v>
       </c>
-      <c r="G102" s="34">
+      <c r="G102">
         <v>2018</v>
       </c>
     </row>
@@ -4115,7 +4051,7 @@
       <c r="C103">
         <v>3</v>
       </c>
-      <c r="G103" s="34">
+      <c r="G103">
         <v>2018</v>
       </c>
     </row>
@@ -4126,7 +4062,7 @@
       <c r="C104">
         <v>4</v>
       </c>
-      <c r="G104" s="34">
+      <c r="G104">
         <v>2018</v>
       </c>
     </row>
@@ -4137,7 +4073,7 @@
       <c r="C105">
         <v>5</v>
       </c>
-      <c r="G105" s="34">
+      <c r="G105">
         <v>2018</v>
       </c>
     </row>
@@ -4152,7 +4088,7 @@
       <c r="D106" s="31"/>
       <c r="E106" s="31"/>
       <c r="F106" s="31"/>
-      <c r="G106" s="37">
+      <c r="G106" s="31">
         <v>2018</v>
       </c>
     </row>
@@ -4166,7 +4102,7 @@
       <c r="C107">
         <v>1</v>
       </c>
-      <c r="G107" s="34">
+      <c r="G107">
         <v>2019</v>
       </c>
     </row>
@@ -4177,7 +4113,7 @@
       <c r="C108" t="s">
         <v>91</v>
       </c>
-      <c r="G108" s="34">
+      <c r="G108">
         <v>2019</v>
       </c>
     </row>
@@ -4188,7 +4124,7 @@
       <c r="C109" t="s">
         <v>92</v>
       </c>
-      <c r="G109" s="34">
+      <c r="G109">
         <v>2019</v>
       </c>
     </row>
@@ -4199,7 +4135,7 @@
       <c r="C110">
         <v>3</v>
       </c>
-      <c r="G110" s="34">
+      <c r="G110">
         <v>2019</v>
       </c>
     </row>
@@ -4210,7 +4146,7 @@
       <c r="C111">
         <v>4</v>
       </c>
-      <c r="G111" s="34">
+      <c r="G111">
         <v>2019</v>
       </c>
     </row>
@@ -4221,7 +4157,7 @@
       <c r="C112">
         <v>5</v>
       </c>
-      <c r="G112" s="34">
+      <c r="G112">
         <v>2019</v>
       </c>
     </row>
@@ -4236,7 +4172,7 @@
       <c r="D113" s="31"/>
       <c r="E113" s="31"/>
       <c r="F113" s="31"/>
-      <c r="G113" s="37">
+      <c r="G113" s="31">
         <v>2019</v>
       </c>
     </row>
@@ -4250,7 +4186,7 @@
       <c r="C114">
         <v>1</v>
       </c>
-      <c r="G114" s="34">
+      <c r="G114">
         <v>2020</v>
       </c>
     </row>
@@ -4261,7 +4197,7 @@
       <c r="C115" t="s">
         <v>91</v>
       </c>
-      <c r="G115" s="34">
+      <c r="G115">
         <v>2020</v>
       </c>
       <c r="I115" t="s">
@@ -4275,7 +4211,7 @@
       <c r="C116" t="s">
         <v>92</v>
       </c>
-      <c r="G116" s="34">
+      <c r="G116">
         <v>2020</v>
       </c>
     </row>
@@ -4286,7 +4222,7 @@
       <c r="C117">
         <v>3</v>
       </c>
-      <c r="G117" s="34">
+      <c r="G117">
         <v>2020</v>
       </c>
     </row>
@@ -4297,7 +4233,7 @@
       <c r="C118">
         <v>4</v>
       </c>
-      <c r="G118" s="34">
+      <c r="G118">
         <v>2020</v>
       </c>
     </row>
@@ -4308,7 +4244,7 @@
       <c r="C119">
         <v>5</v>
       </c>
-      <c r="G119" s="34">
+      <c r="G119">
         <v>2020</v>
       </c>
     </row>
@@ -4323,7 +4259,7 @@
       <c r="D120" s="31"/>
       <c r="E120" s="31"/>
       <c r="F120" s="31"/>
-      <c r="G120" s="37">
+      <c r="G120" s="31">
         <v>2020</v>
       </c>
     </row>
@@ -4340,7 +4276,7 @@
       <c r="D121">
         <v>10</v>
       </c>
-      <c r="G121" s="34">
+      <c r="G121">
         <v>2021</v>
       </c>
     </row>
@@ -4354,7 +4290,7 @@
       <c r="D122">
         <v>1</v>
       </c>
-      <c r="G122" s="34">
+      <c r="G122">
         <v>2021</v>
       </c>
     </row>
@@ -4368,7 +4304,7 @@
       <c r="D123">
         <v>1</v>
       </c>
-      <c r="G123" s="34">
+      <c r="G123">
         <v>2021</v>
       </c>
     </row>
@@ -4382,7 +4318,7 @@
       <c r="D124">
         <v>2</v>
       </c>
-      <c r="G124" s="34">
+      <c r="G124">
         <v>2021</v>
       </c>
     </row>
@@ -4396,7 +4332,7 @@
       <c r="D125">
         <v>0</v>
       </c>
-      <c r="G125" s="34">
+      <c r="G125">
         <v>2021</v>
       </c>
     </row>
@@ -4410,7 +4346,7 @@
       <c r="D126">
         <v>0</v>
       </c>
-      <c r="G126" s="34">
+      <c r="G126">
         <v>2021</v>
       </c>
     </row>
@@ -4425,7 +4361,7 @@
       <c r="D127" s="31"/>
       <c r="E127" s="31"/>
       <c r="F127" s="31"/>
-      <c r="G127" s="37">
+      <c r="G127" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -4439,11 +4375,10 @@
       <c r="C128">
         <v>1</v>
       </c>
-      <c r="D128" s="34">
+      <c r="D128">
         <v>16</v>
       </c>
-      <c r="E128" s="34"/>
-      <c r="G128" s="34">
+      <c r="G128">
         <v>2022</v>
       </c>
     </row>
@@ -4454,11 +4389,10 @@
       <c r="C129" t="s">
         <v>91</v>
       </c>
-      <c r="D129" s="34">
-        <v>0</v>
-      </c>
-      <c r="E129" s="34"/>
-      <c r="G129" s="34">
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="G129">
         <v>2022</v>
       </c>
     </row>
@@ -4469,11 +4403,10 @@
       <c r="C130" t="s">
         <v>92</v>
       </c>
-      <c r="D130" s="34">
+      <c r="D130">
         <v>1</v>
       </c>
-      <c r="E130" s="34"/>
-      <c r="G130" s="34">
+      <c r="G130">
         <v>2022</v>
       </c>
     </row>
@@ -4484,11 +4417,10 @@
       <c r="C131">
         <v>3</v>
       </c>
-      <c r="D131" s="34">
+      <c r="D131">
         <v>1</v>
       </c>
-      <c r="E131" s="34"/>
-      <c r="G131" s="34">
+      <c r="G131">
         <v>2022</v>
       </c>
     </row>
@@ -4499,11 +4431,10 @@
       <c r="C132">
         <v>4</v>
       </c>
-      <c r="D132" s="34">
-        <v>0</v>
-      </c>
-      <c r="E132" s="34"/>
-      <c r="G132" s="34">
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="G132">
         <v>2022</v>
       </c>
     </row>
@@ -4514,26 +4445,25 @@
       <c r="C133">
         <v>5</v>
       </c>
-      <c r="D133" s="34">
-        <v>0</v>
-      </c>
-      <c r="E133" s="34"/>
-      <c r="G133" s="34">
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="G133">
         <v>2022</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" s="39"/>
-      <c r="B134" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C134" s="39">
+      <c r="A134" s="31"/>
+      <c r="B134" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="31">
         <v>6</v>
       </c>
-      <c r="D134" s="39"/>
-      <c r="E134" s="39"/>
-      <c r="F134" s="39"/>
-      <c r="G134" s="40">
+      <c r="D134" s="31"/>
+      <c r="E134" s="31"/>
+      <c r="F134" s="31"/>
+      <c r="G134" s="31">
         <v>2022</v>
       </c>
     </row>
@@ -4547,16 +4477,16 @@
       <c r="C135">
         <v>1</v>
       </c>
-      <c r="D135" s="38">
+      <c r="D135">
         <v>19</v>
       </c>
-      <c r="E135" s="38">
+      <c r="E135">
         <v>18</v>
       </c>
-      <c r="F135" s="38">
+      <c r="F135">
         <v>15</v>
       </c>
-      <c r="G135" s="34">
+      <c r="G135">
         <v>2023</v>
       </c>
     </row>
@@ -4567,14 +4497,13 @@
       <c r="C136" t="s">
         <v>91</v>
       </c>
-      <c r="D136" s="38">
+      <c r="D136">
         <v>1</v>
       </c>
-      <c r="E136" s="38"/>
       <c r="F136">
         <v>1</v>
       </c>
-      <c r="G136" s="34">
+      <c r="G136">
         <v>2023</v>
       </c>
     </row>
@@ -4585,14 +4514,13 @@
       <c r="C137" t="s">
         <v>92</v>
       </c>
-      <c r="D137" s="38">
+      <c r="D137">
         <v>2</v>
       </c>
-      <c r="E137" s="38"/>
       <c r="F137">
         <v>2</v>
       </c>
-      <c r="G137" s="34">
+      <c r="G137">
         <v>2023</v>
       </c>
     </row>
@@ -4603,11 +4531,10 @@
       <c r="C138">
         <v>3</v>
       </c>
-      <c r="D138" s="38">
+      <c r="D138">
         <v>1</v>
       </c>
-      <c r="E138" s="38"/>
-      <c r="G138" s="34">
+      <c r="G138">
         <v>2023</v>
       </c>
     </row>
@@ -4618,11 +4545,10 @@
       <c r="C139">
         <v>4</v>
       </c>
-      <c r="D139" s="38">
-        <v>0</v>
-      </c>
-      <c r="E139" s="38"/>
-      <c r="G139" s="34">
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="G139">
         <v>2023</v>
       </c>
     </row>
@@ -4633,11 +4559,10 @@
       <c r="C140">
         <v>5</v>
       </c>
-      <c r="D140" s="38">
-        <v>0</v>
-      </c>
-      <c r="E140" s="38"/>
-      <c r="G140" s="34">
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="G140">
         <v>2023</v>
       </c>
     </row>
@@ -4654,7 +4579,7 @@
       </c>
       <c r="E141" s="31"/>
       <c r="F141" s="31"/>
-      <c r="G141" s="37">
+      <c r="G141" s="31">
         <v>2023</v>
       </c>
     </row>
@@ -4668,7 +4593,7 @@
       <c r="C142">
         <v>1</v>
       </c>
-      <c r="G142" s="34">
+      <c r="G142">
         <v>2024</v>
       </c>
     </row>
@@ -4679,7 +4604,7 @@
       <c r="C143" t="s">
         <v>91</v>
       </c>
-      <c r="G143" s="34">
+      <c r="G143">
         <v>2024</v>
       </c>
     </row>
@@ -4690,7 +4615,7 @@
       <c r="C144" t="s">
         <v>92</v>
       </c>
-      <c r="G144" s="34">
+      <c r="G144">
         <v>2024</v>
       </c>
     </row>
@@ -4701,7 +4626,7 @@
       <c r="C145">
         <v>3</v>
       </c>
-      <c r="G145" s="34">
+      <c r="G145">
         <v>2024</v>
       </c>
     </row>
@@ -4712,7 +4637,7 @@
       <c r="C146">
         <v>4</v>
       </c>
-      <c r="G146" s="34">
+      <c r="G146">
         <v>2024</v>
       </c>
     </row>
@@ -4723,7 +4648,7 @@
       <c r="C147">
         <v>5</v>
       </c>
-      <c r="G147" s="34">
+      <c r="G147">
         <v>2024</v>
       </c>
     </row>
@@ -4738,7 +4663,7 @@
       <c r="D148" s="31"/>
       <c r="E148" s="31"/>
       <c r="F148" s="31"/>
-      <c r="G148" s="37">
+      <c r="G148" s="31">
         <v>2024</v>
       </c>
     </row>
@@ -4752,7 +4677,7 @@
       <c r="C149">
         <v>1</v>
       </c>
-      <c r="G149" s="34">
+      <c r="G149">
         <v>2025</v>
       </c>
     </row>
@@ -4766,7 +4691,7 @@
       <c r="D150">
         <v>1</v>
       </c>
-      <c r="G150" s="34">
+      <c r="G150">
         <v>2025</v>
       </c>
     </row>
@@ -4777,7 +4702,7 @@
       <c r="C151" t="s">
         <v>92</v>
       </c>
-      <c r="G151" s="34">
+      <c r="G151">
         <v>2025</v>
       </c>
     </row>
@@ -4791,7 +4716,7 @@
       <c r="D152">
         <v>1</v>
       </c>
-      <c r="G152" s="34">
+      <c r="G152">
         <v>2025</v>
       </c>
       <c r="I152" t="s">
@@ -4805,7 +4730,7 @@
       <c r="C153">
         <v>4</v>
       </c>
-      <c r="G153" s="34">
+      <c r="G153">
         <v>2025</v>
       </c>
     </row>
@@ -4819,7 +4744,7 @@
       <c r="D154">
         <v>8</v>
       </c>
-      <c r="G154" s="34">
+      <c r="G154">
         <v>2025</v>
       </c>
     </row>
@@ -4830,7 +4755,7 @@
       <c r="C155">
         <v>6</v>
       </c>
-      <c r="G155" s="34">
+      <c r="G155">
         <v>2025</v>
       </c>
     </row>

</xml_diff>